<commit_message>
match for all responses
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Url request string</t>
   </si>
   <si>
-    <t>Url params</t>
+    <t>Uri params</t>
   </si>
   <si>
     <t>Response</t>
@@ -25,6 +25,36 @@
     <t>Match for all</t>
   </si>
   <si>
+    <t>Match by params</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api?page=1&amp;stream=false</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api?page=1&amp;stream=true</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api?page=2&amp;stream=false</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/api?page=1&amp;stream=false</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/api?page=1&amp;stream=true</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/api?page=2&amp;stream=false</t>
+  </si>
+  <si>
+    <t>http://localhost:3002/api?page=1&amp;stream=false</t>
+  </si>
+  <si>
+    <t>http://localhost:3002/api?page=1&amp;stream=true</t>
+  </si>
+  <si>
+    <t>http://localhost:3002/api?page=2&amp;stream=false</t>
+  </si>
+  <si>
     <t>page=1, stream=false</t>
   </si>
   <si>
@@ -32,15 +62,6 @@
   </si>
   <si>
     <t>page=2, stream=false</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/api?page=1&amp;stream=false</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/api?page=1&amp;stream=true</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/api?page=2&amp;stream=false</t>
   </si>
   <si>
     <t>[object Object],[object Object]</t>
@@ -92,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -102,9 +123,10 @@
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -117,41 +139,110 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dirty match checking
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Url request string</t>
   </si>
@@ -74,6 +74,21 @@
   </si>
   <si>
     <t>Ответы не совпали</t>
+  </si>
+  <si>
+    <t>page=1&amp;stream=false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>page=1&amp;stream=true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>page=2&amp;stream=false</t>
   </si>
 </sst>
 </file>
@@ -113,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -143,7 +158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -156,8 +171,14 @@
       <c r="D2" s="0" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
@@ -167,8 +188,14 @@
       <c r="C3" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
@@ -177,6 +204,12 @@
       </c>
       <c r="C4" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">

</xml_diff>